<commit_message>
Atualização automática de SAO_JOSE_DO_OURO.xlsx
</commit_message>
<xml_diff>
--- a/SAO_JOSE_DO_OURO.xlsx
+++ b/SAO_JOSE_DO_OURO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{09D72EF8-83E0-4908-B8AB-16DC2F3260EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{46725557-9C28-48C2-BD8F-16F5CD82B861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1197,7 +1197,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{50B5FE99-F9C5-4D57-90D8-25728CA8B32C}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{F561DC26-F20B-40FC-8D5A-9302C662F4A7}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1227,10 +1227,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFDDA44F-D215-45AA-9A42-AC11326AC32F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6740B22-2DAF-454C-B9FE-27C945372B79}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1268,7 +1268,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{526DC9E5-CA75-4F8E-9A0D-B721692FDD0A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF786A32-8A90-4138-86A6-F3F780F2EDB3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1331,7 +1331,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B85C6E6-1513-4EA1-9974-2E97B84705CE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED5B35B5-93C0-4864-AB33-CD405FB8366A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1350,7 +1350,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14D015EC-3918-F788-0650-269535380717}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E2F3411-ABAD-C980-E2FD-B24979F8A3C4}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1399,7 +1399,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1B36204-6DE5-9EDE-AF6F-8F478C86F1D4}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D2E3B69-E4A3-C82F-6D52-22A3B9AE20D5}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1418,7 +1418,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{189C841B-A9A1-784F-F56C-8612B6958A67}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1330347-C646-8A4B-7279-4B9E80C2B650}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1449,7 +1449,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{696DBBB5-57E0-45B3-3677-EF04E8E92C9A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91B7BC6F-D4F4-3800-A3AE-FBFB9639E58F}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1480,7 +1480,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B34BE361-1AD3-361D-076A-8D2905D24A63}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD75D198-9009-CADE-50EA-44F6F1219B17}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1523,7 +1523,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D6648DB-4BDC-4433-ADF8-5277BF8C387B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{788DE38A-32DB-4B3F-9D17-995236A51AD7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1561,7 +1561,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{638CADED-4534-4536-9213-825FEFF21B27}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4ECAD73E-8284-4FDA-947A-FA240D57723E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1604,7 +1604,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22060B88-8948-4703-A753-76AC2E7E6CF7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81B81DA5-3BCF-470D-889D-F33FB6876098}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1917,7 +1917,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3F7B598-932D-4C1E-974B-D80EEBE5B48B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{757E2468-4C43-449A-AA39-58A9D7A4C2AB}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>